<commit_message>
air sensor, can show value from sensor, can't calculate mean value from sensor
</commit_message>
<xml_diff>
--- a/voltage_sensor/voltage_sensor_calibration.xlsx
+++ b/voltage_sensor/voltage_sensor_calibration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\Coding\Arduino\cyber physical system and sensor\voltage_sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\Coding\Arduino\cyber_physical_system_and_sensor\voltage_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56B384F-6B96-43FF-BD7A-F1E9F4C66CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6E4343-6578-497A-86DA-9B2D9020E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D4AB3BFD-3C6A-478F-B578-3525CC8FFF7F}"/>
   </bookViews>
@@ -3431,8 +3431,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -9439,7 +9438,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
current, full water proof, metal inductive
</commit_message>
<xml_diff>
--- a/voltage_sensor/voltage_sensor_calibration.xlsx
+++ b/voltage_sensor/voltage_sensor_calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\Coding\Arduino\cyber_physical_system_and_sensor\voltage_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6E4343-6578-497A-86DA-9B2D9020E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2137368-0EAC-4E8A-9A77-6396FB6C0C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D4AB3BFD-3C6A-478F-B578-3525CC8FFF7F}"/>
+    <workbookView xWindow="2505" yWindow="2415" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D4AB3BFD-3C6A-478F-B578-3525CC8FFF7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Calibration" sheetId="1" r:id="rId1"/>
@@ -9437,7 +9437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0741F0-3E2F-47CB-83DC-5C874A7BBF54}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>